<commit_message>
Updated parser logic and frontend components; also modified Excel template
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A6B62B-25DA-475D-A1A1-AB60D99C143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1139D3E9-8D21-4502-B7DA-326F8871A547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="3012" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t>T</t>
   </si>
@@ -212,12 +212,6 @@
   </si>
   <si>
     <t>Program Type</t>
-  </si>
-  <si>
-    <t>Exam Type Code</t>
-  </si>
-  <si>
-    <t>MIDTERM_1/2025</t>
   </si>
   <si>
     <t>Date</t>
@@ -281,6 +275,9 @@
   </si>
   <si>
     <t>application</t>
+  </si>
+  <si>
+    <t>Exam Type</t>
   </si>
 </sst>
 </file>
@@ -670,7 +667,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,7 +711,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="B3" t="str">
         <f ca="1">VLOOKUP(Q3,P6:R17,2,FALSE)</f>
@@ -728,15 +725,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
       <c r="P5" t="s">
         <v>4</v>
       </c>
@@ -749,10 +744,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -765,12 +760,6 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
       <c r="P7">
         <v>2</v>
       </c>
@@ -782,6 +771,12 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="P8">
         <v>3</v>
       </c>
@@ -794,10 +789,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="P9">
         <v>4</v>
@@ -811,10 +806,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="P10">
         <v>5</v>
@@ -827,12 +822,6 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="P11">
         <v>6</v>
       </c>
@@ -844,6 +833,13 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3">
+        <f>DATE(2025,6,10)</f>
+        <v>45818</v>
+      </c>
       <c r="P12">
         <v>7</v>
       </c>
@@ -856,11 +852,15 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="3">
-        <f>DATE(2025,6,10)</f>
-        <v>45818</v>
+        <v>59</v>
+      </c>
+      <c r="B13" s="5">
+        <f>TIME(9,0,0)</f>
+        <v>0.375</v>
+      </c>
+      <c r="C13" s="5">
+        <f>TIME(12,0,0)</f>
+        <v>0.5</v>
       </c>
       <c r="P13">
         <v>8</v>
@@ -873,17 +873,6 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="5">
-        <f>TIME(9,0,0)</f>
-        <v>0.375</v>
-      </c>
-      <c r="C14" s="5">
-        <f>TIME(12,0,0)</f>
-        <v>0.5</v>
-      </c>
       <c r="P14">
         <v>9</v>
       </c>
@@ -969,7 +958,7 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
@@ -1035,31 +1024,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" t="s">
-        <v>66</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1107,10 +1096,10 @@
     </row>
     <row r="3" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>27</v>
@@ -1118,7 +1107,7 @@
     </row>
     <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1322,14 +1311,14 @@
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1343,7 +1332,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1358,30 +1347,30 @@
     </row>
     <row r="4" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
-        <v>76</v>
+      <c r="D4" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
first page UI fixed
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assumption University\Senior Project 1\SeniorProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bella\Desktop\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E91C61-0510-4031-BD01-1594A77030DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C4C099-3348-4532-8E88-BB5258635408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -373,7 +373,7 @@
     <t>hehe.png</t>
   </si>
   <si>
-    <t>BigTower</t>
+    <t>Big Tower</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45831</v>
+        <v>45832</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finally matching randomization fixed
i can rest peacefully now
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assumption University\Senior Project 1\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1139D3E9-8D21-4502-B7DA-326F8871A547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14932FA-2ABA-4D82-AAC7-6EEC050824F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3012" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="5508" yWindow="1104" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
   <si>
     <t>T</t>
   </si>
@@ -278,6 +278,21 @@
   </si>
   <si>
     <t>Exam Type</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>temperature</t>
   </si>
 </sst>
 </file>
@@ -666,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265C5A11-7470-47F7-A597-D724F2E196D1}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -690,7 +705,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45816</v>
+        <v>45826</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1176,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFE4AC3-D33B-41F7-AFE1-650B291E6FA6}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,10 +1247,26 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
Can select categories now
yippie
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assumption University\Senior Project 1\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14932FA-2ABA-4D82-AAC7-6EEC050824F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E91C61-0510-4031-BD01-1594A77030DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5508" yWindow="1104" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
   <si>
     <t>T</t>
   </si>
@@ -293,6 +293,87 @@
   </si>
   <si>
     <t>temperature</t>
+  </si>
+  <si>
+    <t>What animal barks?</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Snake</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>All of the Above</t>
+  </si>
+  <si>
+    <t>Where is Chao Phara River</t>
+  </si>
+  <si>
+    <t>Bkk</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Your Home</t>
+  </si>
+  <si>
+    <t>gg.png</t>
+  </si>
+  <si>
+    <t>kk.png</t>
+  </si>
+  <si>
+    <t>What is Eiffle Tower?</t>
+  </si>
+  <si>
+    <t>Your Grandpa</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Nitrosomonous</t>
+  </si>
+  <si>
+    <t>Nitrobacter</t>
+  </si>
+  <si>
+    <t>jj.png</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>What is the worst fruit ever?</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>Durian</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Starfish</t>
+  </si>
+  <si>
+    <t>hehe.png</t>
+  </si>
+  <si>
+    <t>BigTower</t>
   </si>
 </sst>
 </file>
@@ -705,7 +786,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45826</v>
+        <v>45831</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -938,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3C1A04-8C9A-4AB3-92D4-9CFE7C63CA0B}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,7 +1086,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1064,6 +1145,122 @@
       </c>
       <c r="I4" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFE4AC3-D33B-41F7-AFE1-650B291E6FA6}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
UI fix for catrgory page and deployment built
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bella\Desktop\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C4C099-3348-4532-8E88-BB5258635408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F05FEC-52EB-48DC-959F-BE88F33F5B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="215">
   <si>
     <t>T</t>
   </si>
@@ -124,9 +124,6 @@
     <t>home</t>
   </si>
   <si>
-    <t>Is an apple a fuit?</t>
-  </si>
-  <si>
     <t>Something sweet.</t>
   </si>
   <si>
@@ -244,13 +241,7 @@
     <t>image</t>
   </si>
   <si>
-    <t>Is a pencil a fuit?</t>
-  </si>
-  <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>Is a banana a fruit?</t>
   </si>
   <si>
     <t>q_type</t>
@@ -374,6 +365,327 @@
   </si>
   <si>
     <t>Big Tower</t>
+  </si>
+  <si>
+    <t>Which of these is typically eaten as a dessert?</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Lettuce</t>
+  </si>
+  <si>
+    <t>dessert.png</t>
+  </si>
+  <si>
+    <t>Which of the following is a beverage?</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Juice</t>
+  </si>
+  <si>
+    <t>Steak</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>juice.png</t>
+  </si>
+  <si>
+    <t>Which is a type of pasta?</t>
+  </si>
+  <si>
+    <t>Spaghetti</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Fried Rice</t>
+  </si>
+  <si>
+    <t>Toast</t>
+  </si>
+  <si>
+    <t>Ice cream</t>
+  </si>
+  <si>
+    <t>pasta.png</t>
+  </si>
+  <si>
+    <t>Which of these is a natural place?</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Cafe</t>
+  </si>
+  <si>
+    <t>forest.png</t>
+  </si>
+  <si>
+    <t>Which is located by the beach?</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Cave</t>
+  </si>
+  <si>
+    <t>Harbor</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>beach.png</t>
+  </si>
+  <si>
+    <t>Which of these is a public park?</t>
+  </si>
+  <si>
+    <t>Greenfield</t>
+  </si>
+  <si>
+    <t>Metro Plaza</t>
+  </si>
+  <si>
+    <t>City Library</t>
+  </si>
+  <si>
+    <t>Train Station</t>
+  </si>
+  <si>
+    <t>Cinema</t>
+  </si>
+  <si>
+    <t>park.png</t>
+  </si>
+  <si>
+    <t>Which of these is a mammal?</t>
+  </si>
+  <si>
+    <t>Shark</t>
+  </si>
+  <si>
+    <t>Frog</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>Eagle</t>
+  </si>
+  <si>
+    <t>Lizard</t>
+  </si>
+  <si>
+    <t>dolphin.png</t>
+  </si>
+  <si>
+    <t>Which animal can fly?</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>bird.png</t>
+  </si>
+  <si>
+    <t>Which of these animals lives in water?</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Horse</t>
+  </si>
+  <si>
+    <t>Elephant</t>
+  </si>
+  <si>
+    <t>frog.png</t>
+  </si>
+  <si>
+    <t>Do chairs typically have four legs?</t>
+  </si>
+  <si>
+    <t>Is a window used for cooking?</t>
+  </si>
+  <si>
+    <t>Is a refrigerator used to keep food cold?</t>
+  </si>
+  <si>
+    <t>Is a stove used to wash clothes?</t>
+  </si>
+  <si>
+    <t>Do you sleep in the bathroom?</t>
+  </si>
+  <si>
+    <t>Do curtains cover windows?</t>
+  </si>
+  <si>
+    <t>Is a sofa used for sitting?</t>
+  </si>
+  <si>
+    <t>Do we store clothes in the oven?</t>
+  </si>
+  <si>
+    <t>Do houses usually have doors?</t>
+  </si>
+  <si>
+    <t>Is a light bulb used for heating food?</t>
+  </si>
+  <si>
+    <t>Water boils at 100 degrees Celsius.</t>
+  </si>
+  <si>
+    <t>science</t>
+  </si>
+  <si>
+    <t>The sun is a planet.</t>
+  </si>
+  <si>
+    <t>Humans have five senses.</t>
+  </si>
+  <si>
+    <t>Sound travels faster than light.</t>
+  </si>
+  <si>
+    <t>Plants make food through photosynthesis.</t>
+  </si>
+  <si>
+    <t>An electron has a positive charge.</t>
+  </si>
+  <si>
+    <t>The human heart has two chambers.</t>
+  </si>
+  <si>
+    <t>Gravity pulls objects toward the Earth.</t>
+  </si>
+  <si>
+    <t>Metal conducts electricity.</t>
+  </si>
+  <si>
+    <t>The moon produces its own light.</t>
+  </si>
+  <si>
+    <t>Mount Everest is the highest mountain in the world.</t>
+  </si>
+  <si>
+    <t>geography</t>
+  </si>
+  <si>
+    <t>The Amazon is a desert.</t>
+  </si>
+  <si>
+    <t>Africa is the largest continent.</t>
+  </si>
+  <si>
+    <t>The Pacific Ocean is the largest ocean.</t>
+  </si>
+  <si>
+    <t>Tokyo is the capital of Japan.</t>
+  </si>
+  <si>
+    <t>The Nile River is in South America.</t>
+  </si>
+  <si>
+    <t>There are 7 continents on Earth.</t>
+  </si>
+  <si>
+    <t>Greenland is smaller than Australia.</t>
+  </si>
+  <si>
+    <t>The equator divides the Earth into north and south.</t>
+  </si>
+  <si>
+    <t>Antarctica is the hottest continent.</t>
+  </si>
+  <si>
+    <t>The Great Wall of China was built in the 20th century.</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>World War II ended in 1945.</t>
+  </si>
+  <si>
+    <t>Julius Caesar was a Roman emperor.</t>
+  </si>
+  <si>
+    <t>The pyramids were built by ancient Egyptians.</t>
+  </si>
+  <si>
+    <t>The internet was invented before the telephone.</t>
+  </si>
+  <si>
+    <t>The Declaration of Independence was signed in 1776.</t>
+  </si>
+  <si>
+    <t>The Berlin Wall fell in 1989.</t>
+  </si>
+  <si>
+    <t>Napoleon was from Germany.</t>
+  </si>
+  <si>
+    <t>The Renaissance began in Italy.</t>
+  </si>
+  <si>
+    <t>Abraham Lincoln was the first U.S. president.</t>
+  </si>
+  <si>
+    <t>Something salty.</t>
+  </si>
+  <si>
+    <t>Soy Sauce</t>
+  </si>
+  <si>
+    <t>Something spicy.</t>
+  </si>
+  <si>
+    <t>Chili</t>
+  </si>
+  <si>
+    <t>Something chewy.</t>
+  </si>
+  <si>
+    <t>Beef Jerky</t>
   </si>
 </sst>
 </file>
@@ -786,7 +1098,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45832</v>
+        <v>45833</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -807,7 +1119,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" t="str">
         <f ca="1">VLOOKUP(Q3,P6:R17,2,FALSE)</f>
@@ -823,10 +1135,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P5" t="s">
         <v>4</v>
@@ -840,10 +1152,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -868,7 +1180,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>19</v>
@@ -888,7 +1200,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P9">
         <v>4</v>
@@ -902,7 +1214,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>20</v>
@@ -930,7 +1242,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3">
         <f>DATE(2025,6,10)</f>
@@ -948,7 +1260,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="5">
         <f>TIME(9,0,0)</f>
@@ -1019,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3C1A04-8C9A-4AB3-92D4-9CFE7C63CA0B}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,213 +1366,474 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>103</v>
+      <c r="I2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>63</v>
-      </c>
-      <c r="F4" t="s">
-        <v>64</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
         <v>65</v>
-      </c>
-      <c r="I4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
         <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" t="s">
-        <v>88</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
         <v>89</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" t="s">
-        <v>94</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
         <v>97</v>
       </c>
-      <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>98</v>
-      </c>
-      <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>109</v>
       </c>
-      <c r="I8" t="s">
-        <v>103</v>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>148</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>165</v>
+      </c>
+      <c r="I17" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1271,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589423D0-50CB-4F3F-82F4-CB353E932D78}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,88 +1869,444 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>208</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>199</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1389,7 +2318,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,68 +2340,92 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="3" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C6" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="7" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -1519,8 +2472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15F7917-4FC8-4FF7-B762-EA8CF8ABB661}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,7 +2492,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -1547,27 +2500,27 @@
     </row>
     <row r="2" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>27</v>
@@ -1575,30 +2528,30 @@
     </row>
     <row r="4" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Small UI changes + Bug fix + Code break down optimization
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bella\Desktop\SeniorProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F05FEC-52EB-48DC-959F-BE88F33F5B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD0B7BA-E92A-45BF-AA4D-01A7AFD49902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45833</v>
+        <v>45854</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="Q3">
         <f ca="1">MONTH(Q1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1333,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3C1A04-8C9A-4AB3-92D4-9CFE7C63CA0B}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1847,7 +1847,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1868,223 +1868,223 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>166</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>167</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>168</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>169</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>170</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>171</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>172</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>173</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>174</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>175</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>176</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>178</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>179</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>180</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>181</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>182</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>183</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>184</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>185</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>186</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2092,10 +2092,10 @@
       <c r="A22" t="s">
         <v>187</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2103,10 +2103,10 @@
       <c r="A23" t="s">
         <v>189</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2114,10 +2114,10 @@
       <c r="A24" t="s">
         <v>190</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2125,10 +2125,10 @@
       <c r="A25" t="s">
         <v>191</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2136,10 +2136,10 @@
       <c r="A26" t="s">
         <v>192</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2147,10 +2147,10 @@
       <c r="A27" t="s">
         <v>193</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2158,10 +2158,10 @@
       <c r="A28" t="s">
         <v>194</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2169,10 +2169,10 @@
       <c r="A29" t="s">
         <v>195</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2180,10 +2180,10 @@
       <c r="A30" t="s">
         <v>196</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2191,10 +2191,10 @@
       <c r="A31" t="s">
         <v>197</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2202,10 +2202,10 @@
       <c r="A32" t="s">
         <v>198</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2213,10 +2213,10 @@
       <c r="A33" t="s">
         <v>200</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2224,10 +2224,10 @@
       <c r="A34" t="s">
         <v>201</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2235,10 +2235,10 @@
       <c r="A35" t="s">
         <v>202</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2246,10 +2246,10 @@
       <c r="A36" t="s">
         <v>203</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2257,10 +2257,10 @@
       <c r="A37" t="s">
         <v>204</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2268,10 +2268,10 @@
       <c r="A38" t="s">
         <v>205</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2279,10 +2279,10 @@
       <c r="A39" t="s">
         <v>206</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2290,10 +2290,10 @@
       <c r="A40" t="s">
         <v>207</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2301,10 +2301,10 @@
       <c r="A41" t="s">
         <v>208</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2315,17 +2315,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFE4AC3-D33B-41F7-AFE1-650B291E6FA6}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="70.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -2339,129 +2339,93 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>209</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>211</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>213</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2472,7 +2436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15F7917-4FC8-4FF7-B762-EA8CF8ABB661}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Navigation UI upgrades and edit page UI fix
</commit_message>
<xml_diff>
--- a/QuestionBank-Template-V1.xlsx
+++ b/QuestionBank-Template-V1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assumption University\Senior Project 1\SeniorProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD0B7BA-E92A-45BF-AA4D-01A7AFD49902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB883464-09DE-481F-97A5-401C66E50122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="217">
   <si>
     <t>T</t>
   </si>
@@ -106,21 +106,9 @@
     <t>Which of the following is a fruit?</t>
   </si>
   <si>
-    <t>Pork</t>
-  </si>
-  <si>
-    <t>Beef</t>
-  </si>
-  <si>
-    <t>Basil</t>
-  </si>
-  <si>
     <t>Apple</t>
   </si>
   <si>
-    <t>None of the Above</t>
-  </si>
-  <si>
     <t>home</t>
   </si>
   <si>
@@ -139,19 +127,7 @@
     <t>Which is your favourite place?</t>
   </si>
   <si>
-    <t>Park</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
     <t>Mall</t>
-  </si>
-  <si>
-    <t>Pool</t>
-  </si>
-  <si>
-    <t>Theater</t>
   </si>
   <si>
     <t>places</t>
@@ -418,9 +394,6 @@
     <t>Burger</t>
   </si>
   <si>
-    <t>Fried Rice</t>
-  </si>
-  <si>
     <t>Toast</t>
   </si>
   <si>
@@ -686,6 +659,39 @@
   </si>
   <si>
     <t>Beef Jerky</t>
+  </si>
+  <si>
+    <t>Applesssssss</t>
+  </si>
+  <si>
+    <t>Basilsssssss</t>
+  </si>
+  <si>
+    <t>Beefsssssss</t>
+  </si>
+  <si>
+    <t>Porksssssssssss</t>
+  </si>
+  <si>
+    <t>None of the Abovesss</t>
+  </si>
+  <si>
+    <t>Parkssssssssss</t>
+  </si>
+  <si>
+    <t>Homesssssss</t>
+  </si>
+  <si>
+    <t>Mallssssssss</t>
+  </si>
+  <si>
+    <t>Poolssssssss</t>
+  </si>
+  <si>
+    <t>Theatersssssss</t>
+  </si>
+  <si>
+    <t>Fried Ric</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1104,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45854</v>
+        <v>45896</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1119,7 +1125,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B3" t="str">
         <f ca="1">VLOOKUP(Q3,P6:R17,2,FALSE)</f>
@@ -1130,15 +1136,15 @@
       </c>
       <c r="Q3">
         <f ca="1">MONTH(Q1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="P5" t="s">
         <v>4</v>
@@ -1152,10 +1158,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -1180,7 +1186,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>19</v>
@@ -1200,7 +1206,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P9">
         <v>4</v>
@@ -1214,7 +1220,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>20</v>
@@ -1242,7 +1248,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3">
         <f>DATE(2025,6,10)</f>
@@ -1260,7 +1266,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5">
         <f>TIME(9,0,0)</f>
@@ -1334,7 +1340,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,7 +1372,7 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
@@ -1377,19 +1383,19 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>207</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -1398,442 +1404,442 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>214</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>215</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>216</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I16" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1870,442 +1876,442 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2341,90 +2347,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2456,7 +2462,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -2464,58 +2470,58 @@
     </row>
     <row r="2" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>